<commit_message>
aggiunto template relazione 2
</commit_message>
<xml_diff>
--- a/LAB2/risultati_syn.xlsx
+++ b/LAB2/risultati_syn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gianl\Desktop\POLITO\SECONDO ANNO\INTEGRATED SYSTEM ARCHITECTURE\Lab_ISA\LAB2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3505FF3-95C2-4EEF-B576-23408F811A8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15190B5B-05CA-4456-9359-1488B2DAEC99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5184" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{92E54845-BEC7-49D1-91E7-C593AFD3A972}"/>
+    <workbookView xWindow="4395" yWindow="1455" windowWidth="21600" windowHeight="11385" xr2:uid="{92E54845-BEC7-49D1-91E7-C593AFD3A972}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -169,10 +169,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -496,309 +496,309 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="H1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="2"/>
       <c r="M1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N1" s="4"/>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="1"/>
-      <c r="S1" s="1" t="s">
+      <c r="Q1" s="2"/>
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
         <v>-0.78</v>
       </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
         <v>-1.52</v>
       </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
         <v>-1.55</v>
       </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2">
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
         <v>-1.52</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
         <v>-1.4</v>
       </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
         <v>-3.89</v>
       </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
         <v>-1.41</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>0.78</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>-0.01</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>1.52</v>
       </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
         <v>1.55</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="1">
         <v>-0.39</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="1">
         <v>1.52</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="1">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>1.4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>-0.05</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>3.89</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>-0.39</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>1.41</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>-0.04</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>0.79</v>
       </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2">
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
         <v>1.94</v>
       </c>
-      <c r="Q4" s="2">
-        <v>0</v>
-      </c>
-      <c r="S4" s="2">
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
         <v>1.57</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="1">
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>1.45</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>-0.01</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>4.28</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>0.01</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>1.45</v>
       </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="S5" s="2">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
         <v>1.64</v>
       </c>
-      <c r="T5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>1.46</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>1.5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>-0.06</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>1.56</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>1.56</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>4047.7</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>4.28</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>4851.6000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>1.45</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>4088.4</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>0.79</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>4924.7</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>1.52</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>4188.2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>1.94</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>5360.4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>1.64</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>5327.7</v>
       </c>
     </row>

</xml_diff>